<commit_message>
Replacing test data files with latest.
</commit_message>
<xml_diff>
--- a/Data Files/AppealNumbers.xlsx
+++ b/Data Files/AppealNumbers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Katalon\Data-Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6776821F-E9DE-4331-8EC4-99C809F647C8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1390E167-8A71-4AD1-A17F-43E2F69DA12D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2304" yWindow="2304" windowWidth="23040" windowHeight="12204" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Appeals" sheetId="2" r:id="rId1"/>
@@ -20,48 +20,60 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
   <si>
     <t>ReferenceNum</t>
   </si>
   <si>
+    <t>W/4003621</t>
+  </si>
+  <si>
+    <t>W/4003622</t>
+  </si>
+  <si>
+    <t>W/4003623</t>
+  </si>
+  <si>
+    <t>W/4003624</t>
+  </si>
+  <si>
+    <t>W/4003625</t>
+  </si>
+  <si>
+    <t>W/4003626</t>
+  </si>
+  <si>
+    <t>W/4003627</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
-    <t>W/4002470</t>
-  </si>
-  <si>
-    <t>W/4002472</t>
-  </si>
-  <si>
-    <t>W/4002476</t>
-  </si>
-  <si>
-    <t>W/4002480</t>
-  </si>
-  <si>
-    <t>W/4002482</t>
-  </si>
-  <si>
-    <t>W/4002486</t>
-  </si>
-  <si>
-    <t>W/4002489</t>
-  </si>
-  <si>
-    <t>W/4002521</t>
-  </si>
-  <si>
-    <t>W/4002526</t>
-  </si>
-  <si>
-    <t>W/4002527</t>
-  </si>
-  <si>
-    <t>W/4002532</t>
-  </si>
-  <si>
-    <t>W/4002536</t>
+    <t>W/4003629</t>
+  </si>
+  <si>
+    <t>W/4003641</t>
+  </si>
+  <si>
+    <t>W/4003642</t>
+  </si>
+  <si>
+    <t>W/4003643</t>
+  </si>
+  <si>
+    <t>W/4003644</t>
+  </si>
+  <si>
+    <t>W/4003645</t>
+  </si>
+  <si>
+    <t>W/4003646</t>
+  </si>
+  <si>
+    <t>W/4003647</t>
+  </si>
+  <si>
+    <t>W/4003648</t>
   </si>
 </sst>
 </file>
@@ -414,78 +426,65 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="13.21875" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>